<commit_message>
Work on mark gui
</commit_message>
<xml_diff>
--- a/Time plan Sem2.xlsx
+++ b/Time plan Sem2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="26">
   <si>
     <t>Client meetings</t>
   </si>
@@ -631,7 +631,7 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1056,8 +1056,12 @@
       <c r="J17" s="20">
         <v>29</v>
       </c>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
+      <c r="K17" s="20">
+        <v>5</v>
+      </c>
+      <c r="L17" s="20">
+        <v>5</v>
+      </c>
       <c r="M17" s="20"/>
       <c r="N17" s="20"/>
       <c r="O17" s="20"/>
@@ -1065,7 +1069,7 @@
       <c r="Q17" s="20"/>
       <c r="R17" s="20">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
importing students from spreadsheet done
</commit_message>
<xml_diff>
--- a/Time plan Sem2.xlsx
+++ b/Time plan Sem2.xlsx
@@ -631,7 +631,7 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1062,14 +1062,16 @@
       <c r="L17" s="20">
         <v>18</v>
       </c>
-      <c r="M17" s="20"/>
+      <c r="M17" s="20">
+        <v>6</v>
+      </c>
       <c r="N17" s="20"/>
       <c r="O17" s="20"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="20">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Changed location for account import
accounts import now gives student id
</commit_message>
<xml_diff>
--- a/Time plan Sem2.xlsx
+++ b/Time plan Sem2.xlsx
@@ -1063,7 +1063,7 @@
         <v>18</v>
       </c>
       <c r="M17" s="20">
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="N17" s="20"/>
       <c r="O17" s="20"/>
@@ -1071,7 +1071,7 @@
       <c r="Q17" s="20"/>
       <c r="R17" s="20">
         <f t="shared" si="0"/>
-        <v>92</v>
+        <v>94.5</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added option to include examinee exe when publishing
</commit_message>
<xml_diff>
--- a/Time plan Sem2.xlsx
+++ b/Time plan Sem2.xlsx
@@ -631,7 +631,7 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1065,13 +1065,15 @@
       <c r="M17" s="20">
         <v>10.5</v>
       </c>
-      <c r="N17" s="20"/>
+      <c r="N17" s="20">
+        <v>6</v>
+      </c>
       <c r="O17" s="20"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="20">
         <f t="shared" si="0"/>
-        <v>94.5</v>
+        <v>100.5</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added installer for program
</commit_message>
<xml_diff>
--- a/Time plan Sem2.xlsx
+++ b/Time plan Sem2.xlsx
@@ -1066,14 +1066,14 @@
         <v>10.5</v>
       </c>
       <c r="N17" s="20">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="O17" s="20"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="20">
         <f t="shared" si="0"/>
-        <v>100.5</v>
+        <v>104.5</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>